<commit_message>
Subindo Documentação atualizada Pós Apontamentos do Marcos
</commit_message>
<xml_diff>
--- a/Docs/Backlog/GRUPO11(Backlog).xlsx
+++ b/Docs/Backlog/GRUPO11(Backlog).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Área de Trabalho\Backup SPTech\queijo-minas\Docs\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/rafael_dsilva_sptech_school/Documents/SPRINT 2 e 3/queijo-minas/Docs/Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF99D01-8B1B-492E-A32F-DA27EC39DE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{EFF99D01-8B1B-492E-A32F-DA27EC39DE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBD767B3-F595-4325-9455-B4C0B58DA683}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{E6DED7F9-F2EA-42C5-A892-207AE9F07EE9}"/>
+    <workbookView xWindow="-46188" yWindow="-8856" windowWidth="46296" windowHeight="25416" xr2:uid="{E6DED7F9-F2EA-42C5-A892-207AE9F07EE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="128">
   <si>
     <t>REQUISITO</t>
   </si>
@@ -421,6 +421,9 @@
   </si>
   <si>
     <t>Sprint3</t>
+  </si>
+  <si>
+    <t>BACKLOG DE REQUISITOS - QUEIJO NO PONTO</t>
   </si>
 </sst>
 </file>
@@ -863,6 +866,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -871,9 +877,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2291,8 +2294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06753D1B-5F95-44E8-8917-CD6094E66D47}">
   <dimension ref="B1:J82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="65" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2304,12 +2307,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B1" s="43">
-        <f ca="1">SUMIF(Planilha1!H3:H36,"SPRINT01",Planilha1!C19)</f>
-        <v>0</v>
-      </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
       <c r="E1" s="37"/>
       <c r="F1" s="37"/>
       <c r="G1" s="37"/>
@@ -3148,9 +3150,7 @@
       <c r="G30" s="29">
         <v>8</v>
       </c>
-      <c r="H30" s="46" t="s">
-        <v>13</v>
-      </c>
+      <c r="H30" s="43"/>
       <c r="I30" s="29" t="s">
         <v>25</v>
       </c>
@@ -3461,11 +3461,11 @@
       <c r="B44"/>
     </row>
     <row r="45" spans="2:10" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="46"/>
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
@@ -4083,6 +4083,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="32844186-265b-4793-912a-671da4ac73b2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080A269BF505ACD4B84A4678488096051" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="922643baae8aa488ed079a979f169c7e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32844186-265b-4793-912a-671da4ac73b2" xmlns:ns4="97232348-304c-4ff8-affc-b0d6bfd913f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f7ae9ba316fd031895f045c1b6e4bc8" ns3:_="" ns4:_="">
     <xsd:import namespace="32844186-265b-4793-912a-671da4ac73b2"/>
@@ -4309,24 +4326,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="32844186-265b-4793-912a-671da4ac73b2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F591CB2-BFDE-4C89-ABD1-8880FCE9BE05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C56CDA7-0192-4410-AAE3-52F8B1686740}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="32844186-265b-4793-912a-671da4ac73b2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6590CB1E-15EA-42DD-A92E-18ACF3B9434E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4343,22 +4361,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C56CDA7-0192-4410-AAE3-52F8B1686740}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="32844186-265b-4793-912a-671da4ac73b2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F591CB2-BFDE-4C89-ABD1-8880FCE9BE05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ajuste estético no Backlog
</commit_message>
<xml_diff>
--- a/Docs/Backlog/GRUPO11(Backlog).xlsx
+++ b/Docs/Backlog/GRUPO11(Backlog).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/rafael_dsilva_sptech_school/Documents/SPRINT 2 e 3/queijo-minas/Docs/Backlog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e58d7da8e46fce06/Documents/Sprint 1-2-3/queijo-minas/Docs/Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{EFF99D01-8B1B-492E-A32F-DA27EC39DE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBD767B3-F595-4325-9455-B4C0B58DA683}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{EFF99D01-8B1B-492E-A32F-DA27EC39DE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{337071AD-18D0-4F02-8387-56B5215BC720}"/>
   <bookViews>
-    <workbookView xWindow="-46188" yWindow="-8856" windowWidth="46296" windowHeight="25416" xr2:uid="{E6DED7F9-F2EA-42C5-A892-207AE9F07EE9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6DED7F9-F2EA-42C5-A892-207AE9F07EE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -766,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -878,6 +878,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2294,13 +2298,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06753D1B-5F95-44E8-8917-CD6094E66D47}">
   <dimension ref="B1:J82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="45.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="71.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="103.88671875" style="1" customWidth="1"/>
     <col min="4" max="9" width="15.5546875" style="6" customWidth="1"/>
     <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
@@ -3453,6 +3457,7 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42"/>
+      <c r="C42" s="47"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43"/>
@@ -3796,7 +3801,7 @@
       <c r="B57" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="48" t="s">
         <v>120</v>
       </c>
       <c r="D57" s="22" t="s">
@@ -4083,20 +4088,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="32844186-265b-4793-912a-671da4ac73b2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="32844186-265b-4793-912a-671da4ac73b2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4327,19 +4332,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F591CB2-BFDE-4C89-ABD1-8880FCE9BE05}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C56CDA7-0192-4410-AAE3-52F8B1686740}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="32844186-265b-4793-912a-671da4ac73b2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C56CDA7-0192-4410-AAE3-52F8B1686740}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F591CB2-BFDE-4C89-ABD1-8880FCE9BE05}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="32844186-265b-4793-912a-671da4ac73b2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
subindo Sprint Backlog da Sprint 3
</commit_message>
<xml_diff>
--- a/Docs/Backlog/GRUPO11(Backlog).xlsx
+++ b/Docs/Backlog/GRUPO11(Backlog).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e58d7da8e46fce06/Documents/Sprint 1-2-3/queijo-minas/Docs/Backlog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/rafael_dsilva_sptech_school/Documents/SPRINT 2 e 3/queijo-minas/Docs/Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{EFF99D01-8B1B-492E-A32F-DA27EC39DE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{337071AD-18D0-4F02-8387-56B5215BC720}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="13_ncr:1_{EFF99D01-8B1B-492E-A32F-DA27EC39DE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65B72C69-E233-4BCB-8CED-ED62DC96FC8A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6DED7F9-F2EA-42C5-A892-207AE9F07EE9}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$2:$I$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$2:$I$40</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,8 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="146">
   <si>
     <t>REQUISITO</t>
   </si>
@@ -424,13 +446,67 @@
   </si>
   <si>
     <t>BACKLOG DE REQUISITOS - QUEIJO NO PONTO</t>
+  </si>
+  <si>
+    <t>SPRINT BACKLOG 3</t>
+  </si>
+  <si>
+    <t>Fluxograma de Suporte</t>
+  </si>
+  <si>
+    <t>Ferramenta visual que organiza processos de atendimento ao cliente</t>
+  </si>
+  <si>
+    <t>Ferramenta de suporte ao cliente par resolução de problemas técnicos</t>
+  </si>
+  <si>
+    <t>Documentação de mudanças e atualizações feitas ao longo do projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todos </t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
+    <t>Modelagem de Dados Atualizado</t>
+  </si>
+  <si>
+    <t>Relatório Técnico</t>
+  </si>
+  <si>
+    <t>Manual de Instalação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site Institucional 100% Funcional </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site Institucional com todas as funcionalidades ativas </t>
+  </si>
+  <si>
+    <t>Tabelas com todos os Relacionamentos (1:1, 1:N, N:1, N:N, Relacionamentos Fortes e Fracos)</t>
+  </si>
+  <si>
+    <t>Transformação de dados em códigos para maior segurança</t>
+  </si>
+  <si>
+    <t>Customização de Relatório</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personalização da Interface </t>
+  </si>
+  <si>
+    <t>Documento que fornece informações sobre a instalação do nosso produto/sistema.</t>
+  </si>
+  <si>
+    <t>Em Andamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,6 +546,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -519,7 +601,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -762,11 +844,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -784,9 +877,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -794,9 +884,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -857,9 +944,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -869,6 +953,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -878,10 +966,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2296,59 +2391,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06753D1B-5F95-44E8-8917-CD6094E66D47}">
-  <dimension ref="B1:J82"/>
+  <dimension ref="B1:K83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C60" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="L73" sqref="L73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="71.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="103.88671875" style="1" customWidth="1"/>
-    <col min="4" max="9" width="15.5546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="76.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="151.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="15.5546875" style="6" customWidth="1"/>
     <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="34" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2359,1096 +2455,1096 @@
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="29" t="s">
+      <c r="D3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="27">
         <v>2</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="27">
         <v>13</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="I3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="29" t="s">
+      <c r="D4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="27">
         <v>3</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="27">
         <v>8</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="29">
-        <v>3</v>
-      </c>
-      <c r="G5" s="29">
-        <v>13</v>
-      </c>
-      <c r="H5" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="27">
+        <v>2</v>
+      </c>
+      <c r="G5" s="27">
+        <v>8</v>
+      </c>
+      <c r="H5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="11" t="s">
+      <c r="I5" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="27">
         <v>3</v>
       </c>
-      <c r="G6" s="29">
-        <v>21</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="11" t="s">
+      <c r="G6" s="27">
+        <v>13</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="29">
-        <v>2</v>
-      </c>
-      <c r="G7" s="29">
-        <v>13</v>
-      </c>
-      <c r="H7" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="27">
+        <v>3</v>
+      </c>
+      <c r="G7" s="27">
+        <v>21</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="29">
-        <v>1</v>
-      </c>
-      <c r="G8" s="29">
-        <v>5</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="27">
+        <v>2</v>
+      </c>
+      <c r="G8" s="27">
+        <v>13</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="27">
         <v>1</v>
       </c>
-      <c r="G9" s="29">
-        <v>13</v>
-      </c>
-      <c r="H9" s="29" t="s">
+      <c r="G9" s="27">
+        <v>5</v>
+      </c>
+      <c r="H9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="11" t="s">
+      <c r="I9" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="27">
         <v>1</v>
       </c>
-      <c r="G10" s="29">
-        <v>21</v>
-      </c>
-      <c r="H10" s="29" t="s">
+      <c r="G10" s="27">
         <v>13</v>
       </c>
-      <c r="I10" s="29" t="s">
+      <c r="H10" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="27">
         <v>1</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="27">
+        <v>21</v>
+      </c>
+      <c r="H11" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="11" t="s">
+      <c r="I11" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="29">
-        <v>2</v>
-      </c>
-      <c r="G12" s="29">
+        <v>42</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="27">
+        <v>1</v>
+      </c>
+      <c r="G12" s="27">
         <v>13</v>
       </c>
-      <c r="H12" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="11" t="s">
+      <c r="H12" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="29">
-        <v>2</v>
-      </c>
-      <c r="G13" s="29">
-        <v>8</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="27">
+        <v>3</v>
+      </c>
+      <c r="G13" s="27">
+        <v>13</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="29">
-        <v>3</v>
-      </c>
-      <c r="G14" s="29">
-        <v>21</v>
-      </c>
-      <c r="H14" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="27">
+        <v>2</v>
+      </c>
+      <c r="G14" s="27">
+        <v>13</v>
+      </c>
+      <c r="H14" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="I14" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="27">
         <v>2</v>
       </c>
-      <c r="G15" s="29">
-        <v>5</v>
-      </c>
-      <c r="H15" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="29" t="s">
+      <c r="G15" s="27">
+        <v>8</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="29">
-        <v>1</v>
-      </c>
-      <c r="G16" s="29">
+        <v>50</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="27">
+        <v>3</v>
+      </c>
+      <c r="G16" s="27">
+        <v>21</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="27">
+        <v>2</v>
+      </c>
+      <c r="G17" s="27">
         <v>5</v>
       </c>
-      <c r="H16" s="29" t="s">
+      <c r="H17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="29">
-        <v>3</v>
-      </c>
-      <c r="G17" s="29">
-        <v>13</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="29" t="s">
+      <c r="I17" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="29">
-        <v>2</v>
-      </c>
-      <c r="G18" s="29">
+        <v>81</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="27">
+        <v>1</v>
+      </c>
+      <c r="G18" s="27">
+        <v>8</v>
+      </c>
+      <c r="H18" s="40"/>
+      <c r="I18" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="27">
+        <v>1</v>
+      </c>
+      <c r="G19" s="27">
+        <v>5</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="27">
+        <v>3</v>
+      </c>
+      <c r="G20" s="27">
         <v>13</v>
       </c>
-      <c r="H18" s="29" t="s">
+      <c r="H20" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="29">
-        <v>2</v>
-      </c>
-      <c r="G19" s="29">
-        <v>8</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="29">
-        <v>2</v>
-      </c>
-      <c r="G20" s="29">
-        <v>13</v>
-      </c>
-      <c r="H20" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="11" t="s">
+      <c r="I20" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="27">
         <v>2</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="27">
         <v>13</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="H21" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="J21" s="11" t="s">
+      <c r="I21" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="27">
         <v>2</v>
       </c>
-      <c r="G22" s="29">
-        <v>21</v>
-      </c>
-      <c r="H22" s="29" t="s">
+      <c r="G22" s="27">
+        <v>8</v>
+      </c>
+      <c r="H22" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="J22" s="11" t="s">
+      <c r="I22" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="27">
         <v>2</v>
       </c>
-      <c r="G23" s="29">
-        <v>8</v>
-      </c>
-      <c r="H23" s="29" t="s">
+      <c r="G23" s="27">
+        <v>13</v>
+      </c>
+      <c r="H23" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J23" s="11" t="s">
+      <c r="I23" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="27">
         <v>2</v>
       </c>
-      <c r="G24" s="29">
-        <v>8</v>
-      </c>
-      <c r="H24" s="29" t="s">
+      <c r="G24" s="27">
+        <v>13</v>
+      </c>
+      <c r="H24" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I24" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="11" t="s">
+      <c r="I24" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="27">
+        <v>2</v>
+      </c>
+      <c r="G25" s="27">
+        <v>8</v>
+      </c>
+      <c r="H25" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="27">
+        <v>2</v>
+      </c>
+      <c r="G26" s="27">
+        <v>13</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="27">
+        <v>2</v>
+      </c>
+      <c r="G27" s="27">
+        <v>8</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="27">
+        <v>2</v>
+      </c>
+      <c r="G28" s="27">
+        <v>21</v>
+      </c>
+      <c r="H28" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" s="27">
+        <v>1</v>
+      </c>
+      <c r="G29" s="27">
+        <v>13</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="27">
+        <v>2</v>
+      </c>
+      <c r="G30" s="27">
+        <v>8</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="27">
+        <v>2</v>
+      </c>
+      <c r="G31" s="27">
+        <v>8</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="27">
+        <v>1</v>
+      </c>
+      <c r="G32" s="27">
+        <v>5</v>
+      </c>
+      <c r="H32" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C33" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="29" t="s">
+      <c r="D33" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F33" s="27">
         <v>2</v>
       </c>
-      <c r="G25" s="29">
+      <c r="G33" s="27">
         <v>13</v>
       </c>
-      <c r="H25" s="29" t="s">
+      <c r="H33" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="29" t="s">
+      <c r="I33" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="J33" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B34" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C34" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D34" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E34" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F34" s="27">
         <v>2</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G34" s="27">
         <v>21</v>
       </c>
-      <c r="H26" s="29" t="s">
+      <c r="H34" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="29" t="s">
+      <c r="I34" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="J34" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B35" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="27">
+        <v>1</v>
+      </c>
+      <c r="G35" s="27">
+        <v>8</v>
+      </c>
+      <c r="H35" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="27">
+        <v>3</v>
+      </c>
+      <c r="G36" s="27">
+        <v>8</v>
+      </c>
+      <c r="H36" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="27">
+        <v>3</v>
+      </c>
+      <c r="G37" s="27">
+        <v>13</v>
+      </c>
+      <c r="H37" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="27">
+        <v>3</v>
+      </c>
+      <c r="G38" s="27">
+        <v>21</v>
+      </c>
+      <c r="H38" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="27">
+        <v>3</v>
+      </c>
+      <c r="G39" s="27">
+        <v>13</v>
+      </c>
+      <c r="H39" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J39" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="29">
-        <v>1</v>
-      </c>
-      <c r="G27" s="29">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="27">
+        <v>2</v>
+      </c>
+      <c r="G40" s="27">
         <v>8</v>
       </c>
-      <c r="H27" s="29" t="s">
+      <c r="H40" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J27" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B28" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="29">
-        <v>3</v>
-      </c>
-      <c r="G28" s="29">
-        <v>13</v>
-      </c>
-      <c r="H28" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I28" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29" s="29">
-        <v>1</v>
-      </c>
-      <c r="G29" s="29">
-        <v>13</v>
-      </c>
-      <c r="H29" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="29">
-        <v>1</v>
-      </c>
-      <c r="G30" s="29">
-        <v>8</v>
-      </c>
-      <c r="H30" s="43"/>
-      <c r="I30" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="29">
-        <v>2</v>
-      </c>
-      <c r="G31" s="29">
-        <v>8</v>
-      </c>
-      <c r="H31" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J31" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="29">
-        <v>2</v>
-      </c>
-      <c r="G32" s="29">
-        <v>8</v>
-      </c>
-      <c r="H32" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I32" s="29" t="s">
+      <c r="I40" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" s="29">
-        <v>3</v>
-      </c>
-      <c r="G33" s="29">
-        <v>8</v>
-      </c>
-      <c r="H33" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I33" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" s="29">
-        <v>3</v>
-      </c>
-      <c r="G34" s="29">
-        <v>13</v>
-      </c>
-      <c r="H34" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I34" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="29">
-        <v>2</v>
-      </c>
-      <c r="G35" s="29">
-        <v>13</v>
-      </c>
-      <c r="H35" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I35" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B36" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="D36" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="29">
-        <v>2</v>
-      </c>
-      <c r="G36" s="29">
-        <v>8</v>
-      </c>
-      <c r="H36" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="D37" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="29">
-        <v>2</v>
-      </c>
-      <c r="G37" s="29">
-        <v>8</v>
-      </c>
-      <c r="H37" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J37" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D38" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38" s="29">
-        <v>1</v>
-      </c>
-      <c r="G38" s="29">
-        <v>5</v>
-      </c>
-      <c r="H38" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I38" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="J38" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B39" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D39" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="29">
-        <v>3</v>
-      </c>
-      <c r="G39" s="29">
-        <v>13</v>
-      </c>
-      <c r="H39" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I39" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="J39" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="D40" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="29">
-        <v>3</v>
-      </c>
-      <c r="G40" s="29">
-        <v>21</v>
-      </c>
-      <c r="H40" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I40" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="J40" s="11" t="s">
+      <c r="J40" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3457,7 +3553,10 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42"/>
-      <c r="C42" s="47"/>
+      <c r="C42" s="41" cm="1">
+        <f t="array" aca="1" ref="C42" ca="1">+C12:CC42</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43"/>
@@ -3466,479 +3565,479 @@
       <c r="B44"/>
     </row>
     <row r="45" spans="2:10" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B45" s="45" t="s">
+      <c r="B45" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="C45" s="45"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="38"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D46" s="28" t="s">
+      <c r="D46" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F46" s="21" t="s">
+      <c r="F46" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G46" s="21" t="s">
+      <c r="G46" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I46" s="21" t="s">
+      <c r="I46" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J46" s="36" t="s">
+      <c r="J46" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="27">
+        <v>1</v>
+      </c>
+      <c r="G47" s="27">
+        <v>5</v>
+      </c>
+      <c r="H47" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B48" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="27">
+        <v>1</v>
+      </c>
+      <c r="G48" s="27">
+        <v>8</v>
+      </c>
+      <c r="H48" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B49" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="27">
+        <v>2</v>
+      </c>
+      <c r="G49" s="27">
+        <v>8</v>
+      </c>
+      <c r="H49" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B50" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" s="27">
+        <v>1</v>
+      </c>
+      <c r="G50" s="27">
+        <v>8</v>
+      </c>
+      <c r="H50" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B51" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="27">
+        <v>2</v>
+      </c>
+      <c r="G51" s="27">
+        <v>13</v>
+      </c>
+      <c r="H51" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I51" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B52" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="27">
+        <v>2</v>
+      </c>
+      <c r="G52" s="27">
+        <v>8</v>
+      </c>
+      <c r="H52" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I52" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B53" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="27">
+        <v>2</v>
+      </c>
+      <c r="G53" s="27">
+        <v>13</v>
+      </c>
+      <c r="H53" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I53" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B54" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C54" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="29" t="s">
+      <c r="D54" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F47" s="29">
+      <c r="F54" s="27">
         <v>2</v>
       </c>
-      <c r="G47" s="29">
+      <c r="G54" s="27">
         <v>8</v>
       </c>
-      <c r="H47" s="29" t="s">
+      <c r="H54" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I47" s="29" t="s">
+      <c r="I54" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J47" s="11" t="s">
+      <c r="J54" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B48" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="29" t="s">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B55" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F48" s="29">
+      <c r="F55" s="27">
         <v>2</v>
       </c>
-      <c r="G48" s="29">
+      <c r="G55" s="27">
         <v>13</v>
       </c>
-      <c r="H48" s="29" t="s">
+      <c r="H55" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I48" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J48" s="11" t="s">
+      <c r="I55" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B49" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="29" t="s">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B56" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F49" s="29">
+      <c r="F56" s="27">
         <v>1</v>
       </c>
-      <c r="G49" s="29">
+      <c r="G56" s="27">
         <v>8</v>
       </c>
-      <c r="H49" s="29" t="s">
+      <c r="H56" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="29" t="s">
+      <c r="I56" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J56" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B57" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="27">
+        <v>2</v>
+      </c>
+      <c r="G57" s="27">
+        <v>21</v>
+      </c>
+      <c r="H57" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I57" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B58" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="27">
+        <v>2</v>
+      </c>
+      <c r="G58" s="27">
+        <v>21</v>
+      </c>
+      <c r="H58" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I58" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J49" s="11" t="s">
+      <c r="J58" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B50" s="11" t="s">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B59" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C59" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D50" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="29" t="s">
+      <c r="D59" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="29">
+      <c r="F59" s="27">
         <v>2</v>
       </c>
-      <c r="G50" s="29">
+      <c r="G59" s="27">
         <v>21</v>
       </c>
-      <c r="H50" s="29" t="s">
+      <c r="H59" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I50" s="29" t="s">
+      <c r="I59" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="J50" s="11" t="s">
+      <c r="J59" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B51" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D51" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" s="29">
-        <v>2</v>
-      </c>
-      <c r="G51" s="29">
-        <v>21</v>
-      </c>
-      <c r="H51" s="29" t="s">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B60" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" s="27">
+        <v>3</v>
+      </c>
+      <c r="G60" s="27">
+        <v>13</v>
+      </c>
+      <c r="H60" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I51" s="29" t="s">
+      <c r="I60" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J51" s="11" t="s">
+      <c r="J60" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B52" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52" s="29">
-        <v>2</v>
-      </c>
-      <c r="G52" s="29">
-        <v>21</v>
-      </c>
-      <c r="H52" s="29" t="s">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B61" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F61" s="27">
+        <v>1</v>
+      </c>
+      <c r="G61" s="27">
+        <v>8</v>
+      </c>
+      <c r="H61" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I52" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="J52" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" s="29">
-        <v>2</v>
-      </c>
-      <c r="G53" s="29">
-        <v>8</v>
-      </c>
-      <c r="H53" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I53" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="J53" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B54" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F54" s="29">
-        <v>1</v>
-      </c>
-      <c r="G54" s="29">
-        <v>5</v>
-      </c>
-      <c r="H54" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I54" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J54" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B55" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F55" s="29">
-        <v>1</v>
-      </c>
-      <c r="G55" s="29">
-        <v>8</v>
-      </c>
-      <c r="H55" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I55" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="J55" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B56" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F56" s="29">
-        <v>2</v>
-      </c>
-      <c r="G56" s="29">
-        <v>8</v>
-      </c>
-      <c r="H56" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I56" s="29" t="s">
+      <c r="I61" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J56" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B57" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C57" s="48" t="s">
-        <v>120</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" s="29">
-        <v>2</v>
-      </c>
-      <c r="G57" s="29">
-        <v>13</v>
-      </c>
-      <c r="H57" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I57" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J57" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B58" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F58" s="29">
-        <v>1</v>
-      </c>
-      <c r="G58" s="29">
-        <v>8</v>
-      </c>
-      <c r="H58" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I58" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="J58" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B59" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F59" s="29">
-        <v>3</v>
-      </c>
-      <c r="G59" s="29">
-        <v>13</v>
-      </c>
-      <c r="H59" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I59" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="J59" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B60" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F60" s="29">
-        <v>2</v>
-      </c>
-      <c r="G60" s="29">
-        <v>13</v>
-      </c>
-      <c r="H60" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I60" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J60" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B61" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D61" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F61" s="29">
-        <v>1</v>
-      </c>
-      <c r="G61" s="29">
-        <v>8</v>
-      </c>
-      <c r="H61" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I61" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J61" s="11" t="s">
+      <c r="J61" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3951,69 +4050,430 @@
     <row r="64" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B64"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B65"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B66"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B67"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B68"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B69"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B70"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B71"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B72"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B73"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B74"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B75"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B76"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B77"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B78"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B79"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B80"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:10" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B67" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C67" s="44"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="36"/>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B68" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F68" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="H68" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I68" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J68" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B69" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E69" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="27">
+        <v>2</v>
+      </c>
+      <c r="G69" s="27">
+        <v>8</v>
+      </c>
+      <c r="H69" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I69" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J69" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B70" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E70" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="27">
+        <v>1</v>
+      </c>
+      <c r="G70" s="27">
+        <v>8</v>
+      </c>
+      <c r="H70" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I70" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J70" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B71" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F71" s="27">
+        <v>1</v>
+      </c>
+      <c r="G71" s="27">
+        <v>5</v>
+      </c>
+      <c r="H71" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I71" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J71" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B72" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" s="27">
+        <v>1</v>
+      </c>
+      <c r="G72" s="27">
+        <v>13</v>
+      </c>
+      <c r="H72" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I72" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J72" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B73" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" s="27">
+        <v>1</v>
+      </c>
+      <c r="G73" s="27">
+        <v>8</v>
+      </c>
+      <c r="H73" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I73" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J73" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B74" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E74" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F74" s="27">
+        <v>1</v>
+      </c>
+      <c r="G74" s="27">
+        <v>5</v>
+      </c>
+      <c r="H74" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I74" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J74" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B75" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" s="27">
+        <v>3</v>
+      </c>
+      <c r="G75" s="27">
+        <v>13</v>
+      </c>
+      <c r="H75" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I75" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J75" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B76" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E76" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" s="27">
+        <v>2</v>
+      </c>
+      <c r="G76" s="27">
+        <v>13</v>
+      </c>
+      <c r="H76" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I76" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="J76" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B77" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F77" s="27">
+        <v>1</v>
+      </c>
+      <c r="G77" s="27">
+        <v>3</v>
+      </c>
+      <c r="H77" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I77" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="J77" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B78" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C78" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="27">
+        <v>3</v>
+      </c>
+      <c r="G78" s="27">
+        <v>21</v>
+      </c>
+      <c r="H78" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I78" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J78" s="50" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B79" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="27">
+        <v>2</v>
+      </c>
+      <c r="G79" s="27">
+        <v>8</v>
+      </c>
+      <c r="H79" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I79" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J79" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B80" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F80" s="27">
+        <v>3</v>
+      </c>
+      <c r="G80" s="27">
+        <v>21</v>
+      </c>
+      <c r="H80" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I80" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J80" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B81"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B82"/>
     </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B83"/>
+      <c r="K83" t="e" cm="1">
+        <f t="array" ref="K83">+#REF!:K85CC81:K83</f>
+        <v>#REF!</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B2:I36" xr:uid="{06753D1B-5F95-44E8-8917-CD6094E66D47}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D28">
-    <sortCondition ref="B3:B28"/>
+  <autoFilter ref="B2:I40" xr:uid="{06753D1B-5F95-44E8-8917-CD6094E66D47}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I40">
+      <sortCondition ref="B2:B36"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B69:J83">
+    <sortCondition ref="B83"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B67:D67"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -4029,55 +4489,55 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="28">
         <v>411</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="28">
         <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="28">
         <v>104</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="28">
         <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="28">
         <v>160</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="28">
         <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="28">
         <v>147</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="28">
         <v>137</v>
       </c>
     </row>
@@ -4088,20 +4548,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="32844186-265b-4793-912a-671da4ac73b2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="32844186-265b-4793-912a-671da4ac73b2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4332,19 +4792,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F591CB2-BFDE-4C89-ABD1-8880FCE9BE05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C56CDA7-0192-4410-AAE3-52F8B1686740}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="32844186-265b-4793-912a-671da4ac73b2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F591CB2-BFDE-4C89-ABD1-8880FCE9BE05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Subindo Sprint Backlog 3 Atualizado 100% 2024
</commit_message>
<xml_diff>
--- a/Docs/Backlog/GRUPO11(Backlog).xlsx
+++ b/Docs/Backlog/GRUPO11(Backlog).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/rafael_dsilva_sptech_school/Documents/SPRINT 2 e 3/queijo-minas/Docs/Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="13_ncr:1_{EFF99D01-8B1B-492E-A32F-DA27EC39DE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65B72C69-E233-4BCB-8CED-ED62DC96FC8A}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{EFF99D01-8B1B-492E-A32F-DA27EC39DE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57652250-3D51-4C61-85EF-8A7BE636B27B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6DED7F9-F2EA-42C5-A892-207AE9F07EE9}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="148">
   <si>
     <t>REQUISITO</t>
   </si>
@@ -500,6 +500,12 @@
   </si>
   <si>
     <t>Em Andamento</t>
+  </si>
+  <si>
+    <t>Atualização da Ferramenta de Gestão Trello</t>
+  </si>
+  <si>
+    <t>Painel de visualização das demandas da Sprint</t>
   </si>
 </sst>
 </file>
@@ -859,7 +865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -957,6 +963,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -966,17 +983,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2074,6 +2081,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -2393,8 +2404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06753D1B-5F95-44E8-8917-CD6094E66D47}">
   <dimension ref="B1:K83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C60" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="L73" sqref="L73"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C64" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2407,11 +2418,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="35"/>
       <c r="F1" s="35"/>
       <c r="G1" s="35"/>
@@ -2745,7 +2756,7 @@
       <c r="C13" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="46" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="27" t="s">
@@ -2796,11 +2807,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="45" t="s">
         <v>48</v>
       </c>
       <c r="D15" s="22" t="s">
@@ -2854,7 +2865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
@@ -2887,7 +2898,7 @@
       <c r="B18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="44" t="s">
         <v>82</v>
       </c>
       <c r="D18" s="20" t="s">
@@ -3091,7 +3102,7 @@
       <c r="C25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="46" t="s">
         <v>41</v>
       </c>
       <c r="E25" s="27" t="s">
@@ -3565,11 +3576,11 @@
       <c r="B44"/>
     </row>
     <row r="45" spans="2:10" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="45"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="50"/>
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
@@ -4057,11 +4068,11 @@
       <c r="B66"/>
     </row>
     <row r="67" spans="2:10" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B67" s="44" t="s">
+      <c r="B67" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="C67" s="44"/>
-      <c r="D67" s="45"/>
+      <c r="C67" s="49"/>
+      <c r="D67" s="50"/>
       <c r="E67" s="15"/>
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
@@ -4363,7 +4374,7 @@
       <c r="B78" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C78" s="46" t="s">
+      <c r="C78" s="43" t="s">
         <v>74</v>
       </c>
       <c r="D78" s="20" t="s">
@@ -4384,7 +4395,7 @@
       <c r="I78" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J78" s="50" t="s">
+      <c r="J78" s="47" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4447,10 +4458,37 @@
       </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B81"/>
+      <c r="B81" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F81" s="27">
+        <v>3</v>
+      </c>
+      <c r="G81" s="27">
+        <v>5</v>
+      </c>
+      <c r="H81" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I81" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J81" s="10" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B82"/>
+      <c r="J82" s="51"/>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B83"/>
@@ -4548,23 +4586,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="32844186-265b-4793-912a-671da4ac73b2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080A269BF505ACD4B84A4678488096051" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="922643baae8aa488ed079a979f169c7e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32844186-265b-4793-912a-671da4ac73b2" xmlns:ns4="97232348-304c-4ff8-affc-b0d6bfd913f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f7ae9ba316fd031895f045c1b6e4bc8" ns3:_="" ns4:_="">
     <xsd:import namespace="32844186-265b-4793-912a-671da4ac73b2"/>
@@ -4791,25 +4812,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F591CB2-BFDE-4C89-ABD1-8880FCE9BE05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="32844186-265b-4793-912a-671da4ac73b2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C56CDA7-0192-4410-AAE3-52F8B1686740}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="32844186-265b-4793-912a-671da4ac73b2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6590CB1E-15EA-42DD-A92E-18ACF3B9434E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4826,4 +4846,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C56CDA7-0192-4410-AAE3-52F8B1686740}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="32844186-265b-4793-912a-671da4ac73b2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F591CB2-BFDE-4C89-ABD1-8880FCE9BE05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>